<commit_message>
add sdp category db and template update
</commit_message>
<xml_diff>
--- a/public/templates/questions_import_template.xlsx
+++ b/public/templates/questions_import_template.xlsx
@@ -162,12 +162,12 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="62.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="73.5"/>
   </cols>
   <sheetData>
@@ -371,33 +371,38 @@
       <c r="D35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="2"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="2"/>
       <c r="D40" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B35" type="list">
-      <formula1>"individual,facility"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D40" type="list">
       <formula1>"text,multiple,single,number"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C36" type="list">
       <formula1>"regular,monthly,quarterly,semi-annual,annual"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B40" type="list">
+      <formula1>"individual,facility,sdp"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>